<commit_message>
chapter 1 and 2
</commit_message>
<xml_diff>
--- a/Brainstorming/Ergebnisse.xlsx
+++ b/Brainstorming/Ergebnisse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Desktop\M1\STI\STI-Repo\Brainstorming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9FA342-B970-471F-ABEB-261A09B6AB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76A211D-42D8-4696-99C7-7FD667538F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="1455" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -881,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>